<commit_message>
cierre 5 May 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #04  ABRIL   2022/CREDITOS  4 CARNES   ZAVALETA   ABRIL  2022.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #04  ABRIL   2022/CREDITOS  4 CARNES   ZAVALETA   ABRIL  2022.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6015" yWindow="330" windowWidth="13905" windowHeight="10920" firstSheet="6" activeTab="6"/>
+    <workbookView xWindow="6015" yWindow="330" windowWidth="13905" windowHeight="10920" firstSheet="6" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="REMISIONES OCTUBRE  2021     " sheetId="4" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="62">
   <si>
     <t>REMISION</t>
   </si>
@@ -272,6 +272,63 @@
   <si>
     <t>taras 18-Abr-22</t>
   </si>
+  <si>
+    <t>13246 C</t>
+  </si>
+  <si>
+    <t>13425 C</t>
+  </si>
+  <si>
+    <t>13429 C</t>
+  </si>
+  <si>
+    <t>13460 C</t>
+  </si>
+  <si>
+    <t>13541 C</t>
+  </si>
+  <si>
+    <t>13652 C</t>
+  </si>
+  <si>
+    <t>13809 C</t>
+  </si>
+  <si>
+    <t>13913 C</t>
+  </si>
+  <si>
+    <t>14009 C</t>
+  </si>
+  <si>
+    <t>14039 C</t>
+  </si>
+  <si>
+    <t>14105 C</t>
+  </si>
+  <si>
+    <t>14255 C</t>
+  </si>
+  <si>
+    <t>14326 C</t>
+  </si>
+  <si>
+    <t>14455 C</t>
+  </si>
+  <si>
+    <t>14471 C</t>
+  </si>
+  <si>
+    <t>14550 C</t>
+  </si>
+  <si>
+    <t>14611 C</t>
+  </si>
+  <si>
+    <t>14681 C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABASTOS DE 4 CANRES  HERRADURA </t>
+  </si>
 </sst>
 </file>
 
@@ -283,7 +340,7 @@
     <numFmt numFmtId="165" formatCode="[$-C0A]d\-mmm\-yy;@"/>
     <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -451,8 +508,53 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="1"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -531,8 +633,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="19">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -748,12 +856,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="158">
+  <cellXfs count="174">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1098,6 +1230,36 @@
     <xf numFmtId="166" fontId="3" fillId="9" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="21" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="22" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="23" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="24" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="7" fillId="14" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="7" fillId="14" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="7" fillId="14" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="7" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="25" fillId="14" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -1800,13 +1962,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>647703</xdr:colOff>
-      <xdr:row>67</xdr:row>
+      <xdr:row>61</xdr:row>
       <xdr:rowOff>152402</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>180974</xdr:colOff>
-      <xdr:row>69</xdr:row>
+      <xdr:row>63</xdr:row>
       <xdr:rowOff>133349</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1853,13 +2015,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>561977</xdr:colOff>
-      <xdr:row>67</xdr:row>
+      <xdr:row>61</xdr:row>
       <xdr:rowOff>123829</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>69</xdr:row>
+      <xdr:row>63</xdr:row>
       <xdr:rowOff>161927</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -14349,10 +14511,10 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:I86"/>
+  <dimension ref="A1:I80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="E59" sqref="E59"/>
+    <sheetView topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -14438,7 +14600,7 @@
         <v>9500</v>
       </c>
       <c r="H4" s="18">
-        <f t="shared" ref="H4:H66" si="0">E4-G4</f>
+        <f t="shared" ref="H4:H60" si="0">E4-G4</f>
         <v>0</v>
       </c>
       <c r="I4" s="2"/>
@@ -15480,7 +15642,7 @@
         <v>7600</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="23">
         <v>44678</v>
       </c>
@@ -15501,7 +15663,7 @@
         <v>1446</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="23">
         <v>44678</v>
       </c>
@@ -15522,7 +15684,7 @@
         <v>1954</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="23">
         <v>44679</v>
       </c>
@@ -15543,7 +15705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="23">
         <v>44679</v>
       </c>
@@ -15564,7 +15726,7 @@
         <v>43123</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="23">
         <v>44679</v>
       </c>
@@ -15585,7 +15747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="23">
         <v>44679</v>
       </c>
@@ -15606,7 +15768,7 @@
         <v>6108</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="23">
         <v>44680</v>
       </c>
@@ -15627,7 +15789,7 @@
         <v>12525</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="23">
         <v>44680</v>
       </c>
@@ -15648,7 +15810,7 @@
         <v>25463</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="23">
         <v>44681</v>
       </c>
@@ -15669,7 +15831,7 @@
         <v>2640</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="23">
         <v>44681</v>
       </c>
@@ -15690,11 +15852,9 @@
         <v>51659</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="23"/>
-      <c r="B59" s="13">
-        <v>340</v>
-      </c>
+      <c r="B59" s="13"/>
       <c r="C59" s="24"/>
       <c r="D59" s="19"/>
       <c r="E59" s="20"/>
@@ -15705,213 +15865,191 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="23"/>
-      <c r="B60" s="13">
-        <v>341</v>
-      </c>
-      <c r="C60" s="24"/>
-      <c r="D60" s="19"/>
-      <c r="E60" s="20"/>
-      <c r="F60" s="21"/>
-      <c r="G60" s="22"/>
-      <c r="H60" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="23"/>
-      <c r="B61" s="13">
-        <v>342</v>
-      </c>
-      <c r="C61" s="24"/>
-      <c r="D61" s="19"/>
-      <c r="E61" s="20"/>
-      <c r="F61" s="21"/>
-      <c r="G61" s="22"/>
-      <c r="H61" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="23"/>
-      <c r="B62" s="13">
-        <v>343</v>
-      </c>
-      <c r="C62" s="24"/>
-      <c r="D62" s="19"/>
-      <c r="E62" s="20"/>
-      <c r="F62" s="21"/>
-      <c r="G62" s="22"/>
-      <c r="H62" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="23"/>
-      <c r="B63" s="13">
-        <v>344</v>
-      </c>
-      <c r="C63" s="24"/>
-      <c r="D63" s="19"/>
-      <c r="E63" s="20"/>
-      <c r="F63" s="21"/>
-      <c r="G63" s="22"/>
-      <c r="H63" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="23"/>
-      <c r="B64" s="13">
-        <v>345</v>
-      </c>
-      <c r="C64" s="24"/>
-      <c r="D64" s="19"/>
-      <c r="E64" s="20"/>
-      <c r="F64" s="21"/>
-      <c r="G64" s="22"/>
-      <c r="H64" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="23"/>
-      <c r="B65" s="13"/>
-      <c r="C65" s="24"/>
-      <c r="D65" s="19"/>
-      <c r="E65" s="20"/>
-      <c r="F65" s="21"/>
-      <c r="G65" s="22"/>
-      <c r="H65" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="31"/>
-      <c r="B66" s="111"/>
-      <c r="C66" s="32"/>
-      <c r="D66" s="33"/>
-      <c r="E66" s="34">
-        <v>0</v>
-      </c>
-      <c r="F66" s="35"/>
-      <c r="G66" s="36"/>
-      <c r="H66" s="29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+    <row r="60" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="31"/>
+      <c r="B60" s="111"/>
+      <c r="C60" s="32"/>
+      <c r="D60" s="33"/>
+      <c r="E60" s="34">
+        <v>0</v>
+      </c>
+      <c r="F60" s="35"/>
+      <c r="G60" s="36"/>
+      <c r="H60" s="29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I60" s="2"/>
+    </row>
+    <row r="61" spans="1:9" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B61" s="37"/>
+      <c r="C61" s="38"/>
+      <c r="D61" s="2"/>
+      <c r="E61" s="39">
+        <f>SUM(E4:E60)</f>
+        <v>938122</v>
+      </c>
+      <c r="F61" s="39"/>
+      <c r="G61" s="39">
+        <f>SUM(G4:G60)</f>
+        <v>655048</v>
+      </c>
+      <c r="H61" s="40">
+        <f>SUM(H4:H60)</f>
+        <v>283074</v>
+      </c>
+      <c r="I61" s="2"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B62" s="37"/>
+      <c r="C62" s="38"/>
+      <c r="D62" s="2"/>
+      <c r="E62" s="41"/>
+      <c r="F62" s="42"/>
+      <c r="G62" s="43"/>
+      <c r="H62" s="44"/>
+      <c r="I62" s="2"/>
+    </row>
+    <row r="63" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B63" s="37"/>
+      <c r="C63" s="38"/>
+      <c r="D63" s="2"/>
+      <c r="E63" s="45" t="s">
+        <v>6</v>
+      </c>
+      <c r="F63" s="42"/>
+      <c r="G63" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="H63" s="44"/>
+      <c r="I63" s="2"/>
+    </row>
+    <row r="64" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B64" s="37"/>
+      <c r="C64" s="38"/>
+      <c r="D64" s="2"/>
+      <c r="E64" s="45"/>
+      <c r="F64" s="42"/>
+      <c r="G64" s="46"/>
+      <c r="H64" s="44"/>
+      <c r="I64" s="2"/>
+    </row>
+    <row r="65" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B65" s="37"/>
+      <c r="C65" s="38"/>
+      <c r="D65" s="2"/>
+      <c r="E65" s="141">
+        <f>E61-G61</f>
+        <v>283074</v>
+      </c>
+      <c r="F65" s="142"/>
+      <c r="G65" s="143"/>
+      <c r="I65" s="2"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B66" s="37"/>
+      <c r="C66" s="38"/>
+      <c r="D66" s="2"/>
+      <c r="E66" s="41"/>
+      <c r="F66" s="42"/>
+      <c r="G66" s="43"/>
       <c r="I66" s="2"/>
     </row>
-    <row r="67" spans="1:9" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B67" s="37"/>
       <c r="C67" s="38"/>
       <c r="D67" s="2"/>
-      <c r="E67" s="39">
-        <f>SUM(E4:E66)</f>
-        <v>938122</v>
-      </c>
-      <c r="F67" s="39"/>
-      <c r="G67" s="39">
-        <f>SUM(G4:G66)</f>
-        <v>655048</v>
-      </c>
-      <c r="H67" s="40">
-        <f>SUM(H4:H66)</f>
-        <v>283074</v>
-      </c>
+      <c r="E67" s="144" t="s">
+        <v>8</v>
+      </c>
+      <c r="F67" s="144"/>
+      <c r="G67" s="144"/>
       <c r="I67" s="2"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B68" s="37"/>
-      <c r="C68" s="38"/>
-      <c r="D68" s="2"/>
-      <c r="E68" s="41"/>
-      <c r="F68" s="42"/>
-      <c r="G68" s="43"/>
-      <c r="H68" s="44"/>
+      <c r="A68" s="122"/>
+      <c r="B68" s="123"/>
+      <c r="C68" s="124"/>
+      <c r="D68" s="125"/>
+      <c r="E68" s="126"/>
+      <c r="F68" s="127"/>
+      <c r="G68" s="128"/>
       <c r="I68" s="2"/>
     </row>
-    <row r="69" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B69" s="37"/>
-      <c r="C69" s="38"/>
-      <c r="D69" s="2"/>
-      <c r="E69" s="45" t="s">
-        <v>6</v>
-      </c>
-      <c r="F69" s="42"/>
-      <c r="G69" s="46" t="s">
-        <v>7</v>
-      </c>
-      <c r="H69" s="44"/>
+    <row r="69" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A69" s="112"/>
+      <c r="B69" s="113"/>
+      <c r="C69" s="114"/>
+      <c r="D69" s="49"/>
+      <c r="E69" s="50"/>
+      <c r="F69" s="51"/>
+      <c r="G69" s="50"/>
+      <c r="H69" s="115"/>
       <c r="I69" s="2"/>
     </row>
-    <row r="70" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="37"/>
-      <c r="C70" s="38"/>
-      <c r="D70" s="2"/>
-      <c r="E70" s="45"/>
-      <c r="F70" s="42"/>
-      <c r="G70" s="46"/>
-      <c r="H70" s="44"/>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" s="129"/>
+      <c r="B70" s="130"/>
+      <c r="C70" s="131"/>
+      <c r="D70" s="132"/>
+      <c r="E70" s="133"/>
+      <c r="F70" s="134"/>
+      <c r="G70" s="135"/>
+      <c r="H70" s="115"/>
       <c r="I70" s="2"/>
     </row>
-    <row r="71" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B71" s="37"/>
-      <c r="C71" s="38"/>
-      <c r="D71" s="2"/>
-      <c r="E71" s="141">
-        <f>E67-G67</f>
-        <v>283074</v>
-      </c>
-      <c r="F71" s="142"/>
-      <c r="G71" s="143"/>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" s="129"/>
+      <c r="B71" s="130"/>
+      <c r="C71" s="131"/>
+      <c r="D71" s="132"/>
+      <c r="E71" s="133"/>
+      <c r="F71" s="134"/>
+      <c r="G71" s="135"/>
+      <c r="H71" s="115"/>
       <c r="I71" s="2"/>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B72" s="37"/>
-      <c r="C72" s="38"/>
-      <c r="D72" s="2"/>
-      <c r="E72" s="41"/>
-      <c r="F72" s="42"/>
-      <c r="G72" s="43"/>
+      <c r="A72" s="129"/>
+      <c r="B72" s="130"/>
+      <c r="C72" s="131"/>
+      <c r="D72" s="132"/>
+      <c r="E72" s="133"/>
+      <c r="F72" s="134"/>
+      <c r="G72" s="135"/>
+      <c r="H72" s="115"/>
       <c r="I72" s="2"/>
     </row>
-    <row r="73" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B73" s="37"/>
-      <c r="C73" s="38"/>
-      <c r="D73" s="2"/>
-      <c r="E73" s="144" t="s">
-        <v>8</v>
-      </c>
-      <c r="F73" s="144"/>
-      <c r="G73" s="144"/>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" s="129"/>
+      <c r="B73" s="130"/>
+      <c r="C73" s="131"/>
+      <c r="D73" s="132"/>
+      <c r="E73" s="133"/>
+      <c r="F73" s="134"/>
+      <c r="G73" s="135"/>
+      <c r="H73" s="115"/>
       <c r="I73" s="2"/>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A74" s="122"/>
-      <c r="B74" s="123"/>
-      <c r="C74" s="124"/>
-      <c r="D74" s="125"/>
-      <c r="E74" s="126"/>
-      <c r="F74" s="127"/>
-      <c r="G74" s="128"/>
+      <c r="A74" s="129"/>
+      <c r="B74" s="130"/>
+      <c r="C74" s="131"/>
+      <c r="D74" s="132"/>
+      <c r="E74" s="133"/>
+      <c r="F74" s="134"/>
+      <c r="G74" s="135"/>
+      <c r="H74" s="115"/>
       <c r="I74" s="2"/>
     </row>
-    <row r="75" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A75" s="112"/>
-      <c r="B75" s="113"/>
-      <c r="C75" s="114"/>
-      <c r="D75" s="49"/>
-      <c r="E75" s="50"/>
-      <c r="F75" s="51"/>
-      <c r="G75" s="50"/>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75" s="129"/>
+      <c r="B75" s="130"/>
+      <c r="C75" s="131"/>
+      <c r="D75" s="132"/>
+      <c r="E75" s="133"/>
+      <c r="F75" s="134"/>
+      <c r="G75" s="135"/>
       <c r="H75" s="115"/>
       <c r="I75" s="2"/>
     </row>
@@ -15957,89 +16095,23 @@
       <c r="F79" s="134"/>
       <c r="G79" s="135"/>
       <c r="H79" s="115"/>
-      <c r="I79" s="2"/>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A80" s="129"/>
-      <c r="B80" s="130"/>
-      <c r="C80" s="131"/>
-      <c r="D80" s="132"/>
-      <c r="E80" s="133"/>
-      <c r="F80" s="134"/>
-      <c r="G80" s="135"/>
+      <c r="A80" s="116"/>
+      <c r="B80" s="117"/>
+      <c r="C80" s="118"/>
+      <c r="D80" s="115"/>
+      <c r="E80" s="119"/>
+      <c r="F80" s="120"/>
+      <c r="G80" s="121"/>
       <c r="H80" s="115"/>
-      <c r="I80" s="2"/>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A81" s="129"/>
-      <c r="B81" s="130"/>
-      <c r="C81" s="131"/>
-      <c r="D81" s="132"/>
-      <c r="E81" s="133"/>
-      <c r="F81" s="134"/>
-      <c r="G81" s="135"/>
-      <c r="H81" s="115"/>
-      <c r="I81" s="2"/>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A82" s="129"/>
-      <c r="B82" s="130"/>
-      <c r="C82" s="131"/>
-      <c r="D82" s="132"/>
-      <c r="E82" s="133"/>
-      <c r="F82" s="134"/>
-      <c r="G82" s="135"/>
-      <c r="H82" s="115"/>
-      <c r="I82" s="2"/>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A83" s="129"/>
-      <c r="B83" s="130"/>
-      <c r="C83" s="131"/>
-      <c r="D83" s="132"/>
-      <c r="E83" s="133"/>
-      <c r="F83" s="134"/>
-      <c r="G83" s="135"/>
-      <c r="H83" s="115"/>
-      <c r="I83" s="2"/>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A84" s="129"/>
-      <c r="B84" s="130"/>
-      <c r="C84" s="131"/>
-      <c r="D84" s="132"/>
-      <c r="E84" s="133"/>
-      <c r="F84" s="134"/>
-      <c r="G84" s="135"/>
-      <c r="H84" s="115"/>
-      <c r="I84" s="2"/>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A85" s="129"/>
-      <c r="B85" s="130"/>
-      <c r="C85" s="131"/>
-      <c r="D85" s="132"/>
-      <c r="E85" s="133"/>
-      <c r="F85" s="134"/>
-      <c r="G85" s="135"/>
-      <c r="H85" s="115"/>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A86" s="116"/>
-      <c r="B86" s="117"/>
-      <c r="C86" s="118"/>
-      <c r="D86" s="115"/>
-      <c r="E86" s="119"/>
-      <c r="F86" s="120"/>
-      <c r="G86" s="121"/>
-      <c r="H86" s="115"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="B2:F2"/>
-    <mergeCell ref="E71:G71"/>
-    <mergeCell ref="E73:G73"/>
+    <mergeCell ref="E65:G65"/>
+    <mergeCell ref="E67:G67"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -16050,13 +16122,366 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" style="53" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="B1" s="173" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="163">
+        <v>44616</v>
+      </c>
+      <c r="B3" s="158" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="22">
+        <v>61856.639999999999</v>
+      </c>
+      <c r="D3" s="167">
+        <v>44643</v>
+      </c>
+      <c r="E3" s="171">
+        <v>61856.639999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="163">
+        <v>44617</v>
+      </c>
+      <c r="B4" s="158" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="22">
+        <v>145889.51999999999</v>
+      </c>
+      <c r="D4" s="167">
+        <v>44643</v>
+      </c>
+      <c r="E4" s="171">
+        <v>145889.51999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="159">
+        <v>44617</v>
+      </c>
+      <c r="B5" s="160" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="22">
+        <v>200</v>
+      </c>
+      <c r="D5" s="167">
+        <v>44643</v>
+      </c>
+      <c r="E5" s="171">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="161">
+        <v>44617</v>
+      </c>
+      <c r="B6" s="162" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="22">
+        <v>2373.8000000000002</v>
+      </c>
+      <c r="D6" s="167">
+        <v>44643</v>
+      </c>
+      <c r="E6" s="171">
+        <v>2373.8000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="161">
+        <v>44618</v>
+      </c>
+      <c r="B7" s="162" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="22">
+        <v>40377.15</v>
+      </c>
+      <c r="D7" s="167">
+        <v>44643</v>
+      </c>
+      <c r="E7" s="171">
+        <v>40377.15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="164">
+        <v>44620</v>
+      </c>
+      <c r="B8" s="165" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="166">
+        <v>2909.4</v>
+      </c>
+      <c r="D8" s="167">
+        <v>44643</v>
+      </c>
+      <c r="E8" s="168">
+        <v>2909.4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="164">
+        <v>44621</v>
+      </c>
+      <c r="B9" s="165" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="166">
+        <v>74016.2</v>
+      </c>
+      <c r="D9" s="167">
+        <v>44643</v>
+      </c>
+      <c r="E9" s="168">
+        <v>74016.2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="164">
+        <v>44622</v>
+      </c>
+      <c r="B10" s="165" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="166">
+        <v>38036.6</v>
+      </c>
+      <c r="D10" s="167">
+        <v>44643</v>
+      </c>
+      <c r="E10" s="168">
+        <v>38036.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="164">
+        <v>44623</v>
+      </c>
+      <c r="B11" s="165" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="166">
+        <v>52111.11</v>
+      </c>
+      <c r="D11" s="167">
+        <v>44643</v>
+      </c>
+      <c r="E11" s="168">
+        <v>52111.11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="164">
+        <v>44623</v>
+      </c>
+      <c r="B12" s="165" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="166">
+        <v>394.2</v>
+      </c>
+      <c r="D12" s="167">
+        <v>44643</v>
+      </c>
+      <c r="E12" s="168">
+        <v>394.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="164">
+        <v>44624</v>
+      </c>
+      <c r="B13" s="165" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="166">
+        <v>52173.7</v>
+      </c>
+      <c r="D13" s="167">
+        <v>44643</v>
+      </c>
+      <c r="E13" s="168">
+        <v>52173.7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="164">
+        <v>44625</v>
+      </c>
+      <c r="B14" s="165" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="166">
+        <v>47563.28</v>
+      </c>
+      <c r="D14" s="167">
+        <v>44643</v>
+      </c>
+      <c r="E14" s="168">
+        <v>47563.28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="164">
+        <v>44625</v>
+      </c>
+      <c r="B15" s="165" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="166">
+        <v>1406</v>
+      </c>
+      <c r="D15" s="167">
+        <v>44643</v>
+      </c>
+      <c r="E15" s="168">
+        <v>1406</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="164">
+        <v>44627</v>
+      </c>
+      <c r="B16" s="165" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" s="166">
+        <v>44449.599999999999</v>
+      </c>
+      <c r="D16" s="167">
+        <v>44643</v>
+      </c>
+      <c r="E16" s="168">
+        <v>44449.599999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="164">
+        <v>44627</v>
+      </c>
+      <c r="B17" s="165" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="166">
+        <v>848.4</v>
+      </c>
+      <c r="D17" s="167">
+        <v>44643</v>
+      </c>
+      <c r="E17" s="168">
+        <v>848.4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="164">
+        <v>44628</v>
+      </c>
+      <c r="B18" s="165" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" s="166">
+        <v>71723.600000000006</v>
+      </c>
+      <c r="D18" s="167">
+        <v>44643</v>
+      </c>
+      <c r="E18" s="168">
+        <v>71723.600000000006</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="164">
+        <v>44628</v>
+      </c>
+      <c r="B19" s="165" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" s="166">
+        <v>1776</v>
+      </c>
+      <c r="D19" s="167">
+        <v>44643</v>
+      </c>
+      <c r="E19" s="168">
+        <v>1776</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="164">
+        <v>44629</v>
+      </c>
+      <c r="B20" s="165" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="166">
+        <v>76124.3</v>
+      </c>
+      <c r="D20" s="167">
+        <v>44643</v>
+      </c>
+      <c r="E20" s="168">
+        <v>61979.8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="161"/>
+      <c r="B21" s="162"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="170"/>
+      <c r="E21" s="169">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="161"/>
+      <c r="B22" s="162"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="170"/>
+      <c r="E22" s="169">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A23" s="161">
+        <v>44618</v>
+      </c>
+      <c r="B23" s="162" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="22"/>
+      <c r="E23" s="172">
+        <f>SUM(E3:E22)</f>
+        <v>700085</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>